<commit_message>
OSII - sum total value of sme item under same location
</commit_message>
<xml_diff>
--- a/Dara's Ice Cream/Wastage/CustomReports/WastageMonthlyReport.xlsx
+++ b/Dara's Ice Cream/Wastage/CustomReports/WastageMonthlyReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="209">
   <si>
     <t>Raw Materials Wastage Cost Centers</t>
   </si>
@@ -32,7 +32,7 @@
     <t>Total Qty</t>
   </si>
   <si>
-    <t>O1 Flagship</t>
+    <t>Zamalek Dara's Ice Cream</t>
   </si>
   <si>
     <t>Bakery</t>
@@ -53,7 +53,109 @@
     <t>Churros - Milk Chocolate (PA)</t>
   </si>
   <si>
-    <t>7.8</t>
+    <t>Churros - Sugar &amp; Cinnamon (PA)</t>
+  </si>
+  <si>
+    <t>Cream Icing Cup Cake - Chocolate (PA)</t>
+  </si>
+  <si>
+    <t>Cream Icing Cup Cake - Vanilla (PA)</t>
+  </si>
+  <si>
+    <t>Crumble Powder Finishing Cup Cake - Chocolate (PA)</t>
+  </si>
+  <si>
+    <t>Cup Cake - Chocolate{PC's} (PA)</t>
+  </si>
+  <si>
+    <t>Cup Cake - Vanilla {PC's} (PA)</t>
+  </si>
+  <si>
+    <t>Dough_Cup Cake - Vanilla (PA)</t>
+  </si>
+  <si>
+    <t>Dough-Cup Cake - Chocolate (PA)</t>
+  </si>
+  <si>
+    <t>F.White Ch. Lotus (PA)</t>
+  </si>
+  <si>
+    <t>fa (PA)</t>
+  </si>
+  <si>
+    <t>Semi_Churros Dough (PA)</t>
+  </si>
+  <si>
+    <t>Sugar &amp; Cinnamon Mix (PA)</t>
+  </si>
+  <si>
+    <t>Outlets Products</t>
+  </si>
+  <si>
+    <t>Almond Caramelized (PA)</t>
+  </si>
+  <si>
+    <t>Almond Crumble (PA)</t>
+  </si>
+  <si>
+    <t>Banana Madness_Ice Cream (PA)</t>
+  </si>
+  <si>
+    <t>Belgian Chocolate_Ice Cream (PA)</t>
+  </si>
+  <si>
+    <t>Blondie_Ice Cream (PA)</t>
+  </si>
+  <si>
+    <t>Brownie Cookies (PA)</t>
+  </si>
+  <si>
+    <t>Brownies_dough (PA)</t>
+  </si>
+  <si>
+    <t>Burnt Toffee _Ice Cream (PA)</t>
+  </si>
+  <si>
+    <t>Caramel Ribbon Truelove_Ice Cream (PA)</t>
+  </si>
+  <si>
+    <t>Caramel Sauce (PA)</t>
+  </si>
+  <si>
+    <t>Caramel Sauce for (ADD) (PA)</t>
+  </si>
+  <si>
+    <t>Caramel&amp;peanut crunches One&amp;Only_Ice Cream (PA)</t>
+  </si>
+  <si>
+    <t>Caramelized almond_Ice Cream (PA)</t>
+  </si>
+  <si>
+    <t>3.421</t>
+  </si>
+  <si>
+    <t>Kilogram</t>
+  </si>
+  <si>
+    <t>0.09</t>
+  </si>
+  <si>
+    <t>Caramelized peanuts_Ice Cream (PA)</t>
+  </si>
+  <si>
+    <t>Chocolate Cake_Ice Cream (PA)</t>
+  </si>
+  <si>
+    <t>Chocolate Caramel Lovebird_Ice Cream (PA)</t>
+  </si>
+  <si>
+    <t>Chocolate Chip Cookies (PA)</t>
+  </si>
+  <si>
+    <t>Chocolate Cone (PA)</t>
+  </si>
+  <si>
+    <t>13.936</t>
   </si>
   <si>
     <t>Each</t>
@@ -62,108 +164,6 @@
     <t>2.0</t>
   </si>
   <si>
-    <t>Churros - Sugar &amp; Cinnamon (PA)</t>
-  </si>
-  <si>
-    <t>Cream Icing Cup Cake - Chocolate (PA)</t>
-  </si>
-  <si>
-    <t>Cream Icing Cup Cake - Vanilla (PA)</t>
-  </si>
-  <si>
-    <t>Crumble Powder Finishing Cup Cake - Chocolate (PA)</t>
-  </si>
-  <si>
-    <t>Cup Cake - Chocolate{PC's} (PA)</t>
-  </si>
-  <si>
-    <t>Cup Cake - Vanilla {PC's} (PA)</t>
-  </si>
-  <si>
-    <t>Dough_Cup Cake - Vanilla (PA)</t>
-  </si>
-  <si>
-    <t>Dough-Cup Cake - Chocolate (PA)</t>
-  </si>
-  <si>
-    <t>F.White Ch. Lotus (PA)</t>
-  </si>
-  <si>
-    <t>fa (PA)</t>
-  </si>
-  <si>
-    <t>Semi_Churros Dough (PA)</t>
-  </si>
-  <si>
-    <t>Sugar &amp; Cinnamon Mix (PA)</t>
-  </si>
-  <si>
-    <t>0.913</t>
-  </si>
-  <si>
-    <t>Kilogram</t>
-  </si>
-  <si>
-    <t>0.125</t>
-  </si>
-  <si>
-    <t>Outlets Products</t>
-  </si>
-  <si>
-    <t>Almond Caramelized (PA)</t>
-  </si>
-  <si>
-    <t>Almond Crumble (PA)</t>
-  </si>
-  <si>
-    <t>Banana Madness_Ice Cream (PA)</t>
-  </si>
-  <si>
-    <t>Belgian Chocolate_Ice Cream (PA)</t>
-  </si>
-  <si>
-    <t>Blondie_Ice Cream (PA)</t>
-  </si>
-  <si>
-    <t>Brownie Cookies (PA)</t>
-  </si>
-  <si>
-    <t>Brownies_dough (PA)</t>
-  </si>
-  <si>
-    <t>Burnt Toffee _Ice Cream (PA)</t>
-  </si>
-  <si>
-    <t>Caramel Ribbon Truelove_Ice Cream (PA)</t>
-  </si>
-  <si>
-    <t>Caramel Sauce (PA)</t>
-  </si>
-  <si>
-    <t>Caramel Sauce for (ADD) (PA)</t>
-  </si>
-  <si>
-    <t>Caramel&amp;peanut crunches One&amp;Only_Ice Cream (PA)</t>
-  </si>
-  <si>
-    <t>Caramelized almond_Ice Cream (PA)</t>
-  </si>
-  <si>
-    <t>Caramelized peanuts_Ice Cream (PA)</t>
-  </si>
-  <si>
-    <t>Chocolate Cake_Ice Cream (PA)</t>
-  </si>
-  <si>
-    <t>Chocolate Caramel Lovebird_Ice Cream (PA)</t>
-  </si>
-  <si>
-    <t>Chocolate Chip Cookies (PA)</t>
-  </si>
-  <si>
-    <t>Chocolate Cone (PA)</t>
-  </si>
-  <si>
     <t>Chocolate Sauce_Kitchen (PA)</t>
   </si>
   <si>
@@ -191,12 +191,6 @@
     <t>Cone_Mix (PA)</t>
   </si>
   <si>
-    <t>45.198</t>
-  </si>
-  <si>
-    <t>0.54</t>
-  </si>
-  <si>
     <t>Dark Cookies (PA)</t>
   </si>
   <si>
@@ -305,6 +299,9 @@
     <t>Salted C.Crunches_Ice Cream (PA)</t>
   </si>
   <si>
+    <t>3.499</t>
+  </si>
+  <si>
     <t>Salted Crunchy (PA)</t>
   </si>
   <si>
@@ -449,6 +446,12 @@
     <t>Cone (PA)</t>
   </si>
   <si>
+    <t>77.25</t>
+  </si>
+  <si>
+    <t>15.0</t>
+  </si>
+  <si>
     <t>Cone dough (PA)</t>
   </si>
   <si>
@@ -608,7 +611,19 @@
     <t>Soft Mix Berry-Ice Cream (PA)</t>
   </si>
   <si>
+    <t>33.679</t>
+  </si>
+  <si>
+    <t>0.73</t>
+  </si>
+  <si>
     <t>Soft Vanilla-Ice Cream (PA)</t>
+  </si>
+  <si>
+    <t>26.829</t>
+  </si>
+  <si>
+    <t>1.34</t>
   </si>
   <si>
     <t>Soft Yoghurt-Ice Cream (PA)</t>
@@ -710,7 +725,7 @@
     <col min="1" max="1" width="62.26171875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.41015625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="13.85546875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="16.890625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="35.6953125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -775,18 +790,18 @@
         <v>12</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s" s="4">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s" s="4">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="4">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s" s="4">
         <v>8</v>
@@ -800,7 +815,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="4">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s" s="4">
         <v>8</v>
@@ -814,7 +829,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="4">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s" s="4">
         <v>8</v>
@@ -828,7 +843,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="4">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s" s="4">
         <v>8</v>
@@ -842,7 +857,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s" s="4">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s" s="4">
         <v>8</v>
@@ -856,7 +871,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s" s="4">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s" s="4">
         <v>8</v>
@@ -870,7 +885,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="4">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s" s="4">
         <v>8</v>
@@ -884,7 +899,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="4">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s" s="4">
         <v>8</v>
@@ -898,7 +913,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="4">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s" s="4">
         <v>8</v>
@@ -912,7 +927,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="4">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s" s="4">
         <v>8</v>
@@ -926,7 +941,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="4">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s" s="4">
         <v>8</v>
@@ -940,21 +955,21 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="4">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s" s="4">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="C19" t="s" s="4">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="D19" t="s" s="4">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="3">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s" s="3">
         <v>8</v>
@@ -968,7 +983,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="4">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s" s="4">
         <v>8</v>
@@ -982,7 +997,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s" s="4">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B22" t="s" s="4">
         <v>8</v>
@@ -996,7 +1011,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="4">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s" s="4">
         <v>8</v>
@@ -1010,7 +1025,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s" s="4">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s" s="4">
         <v>8</v>
@@ -1024,7 +1039,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="4">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s" s="4">
         <v>8</v>
@@ -1038,7 +1053,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="4">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s" s="4">
         <v>8</v>
@@ -1052,7 +1067,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="4">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B27" t="s" s="4">
         <v>8</v>
@@ -1066,7 +1081,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="4">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s" s="4">
         <v>8</v>
@@ -1080,7 +1095,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s" s="4">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B29" t="s" s="4">
         <v>8</v>
@@ -1094,7 +1109,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="4">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B30" t="s" s="4">
         <v>8</v>
@@ -1108,7 +1123,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="4">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B31" t="s" s="4">
         <v>8</v>
@@ -1122,7 +1137,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s" s="4">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B32" t="s" s="4">
         <v>8</v>
@@ -1136,21 +1151,21 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="4">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B33" t="s" s="4">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C33" t="s" s="4">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D33" t="s" s="4">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="4">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B34" t="s" s="4">
         <v>8</v>
@@ -1164,7 +1179,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="4">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B35" t="s" s="4">
         <v>8</v>
@@ -1178,7 +1193,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="4">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B36" t="s" s="4">
         <v>8</v>
@@ -1192,7 +1207,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="4">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B37" t="s" s="4">
         <v>8</v>
@@ -1206,16 +1221,16 @@
     </row>
     <row r="38">
       <c r="A38" t="s" s="4">
+        <v>46</v>
+      </c>
+      <c r="B38" t="s" s="4">
+        <v>48</v>
+      </c>
+      <c r="C38" t="s" s="4">
         <v>49</v>
       </c>
-      <c r="B38" t="s" s="4">
-        <v>8</v>
-      </c>
-      <c r="C38" t="s" s="4">
-        <v>11</v>
-      </c>
       <c r="D38" t="s" s="4">
-        <v>10</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39">
@@ -1335,18 +1350,18 @@
         <v>58</v>
       </c>
       <c r="B47" t="s" s="4">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="C47" t="s" s="4">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="D47" t="s" s="4">
-        <v>59</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="4">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B48" t="s" s="4">
         <v>8</v>
@@ -1360,7 +1375,7 @@
     </row>
     <row r="49">
       <c r="A49" t="s" s="4">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B49" t="s" s="4">
         <v>8</v>
@@ -1374,7 +1389,7 @@
     </row>
     <row r="50">
       <c r="A50" t="s" s="4">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B50" t="s" s="4">
         <v>8</v>
@@ -1388,7 +1403,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="4">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B51" t="s" s="4">
         <v>8</v>
@@ -1402,7 +1417,7 @@
     </row>
     <row r="52">
       <c r="A52" t="s" s="4">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B52" t="s" s="4">
         <v>8</v>
@@ -1416,7 +1431,7 @@
     </row>
     <row r="53">
       <c r="A53" t="s" s="4">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B53" t="s" s="4">
         <v>8</v>
@@ -1430,7 +1445,7 @@
     </row>
     <row r="54">
       <c r="A54" t="s" s="4">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B54" t="s" s="4">
         <v>8</v>
@@ -1444,7 +1459,7 @@
     </row>
     <row r="55">
       <c r="A55" t="s" s="4">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B55" t="s" s="4">
         <v>8</v>
@@ -1458,7 +1473,7 @@
     </row>
     <row r="56">
       <c r="A56" t="s" s="4">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B56" t="s" s="4">
         <v>8</v>
@@ -1472,7 +1487,7 @@
     </row>
     <row r="57">
       <c r="A57" t="s" s="4">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B57" t="s" s="4">
         <v>8</v>
@@ -1486,7 +1501,7 @@
     </row>
     <row r="58">
       <c r="A58" t="s" s="4">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B58" t="s" s="4">
         <v>8</v>
@@ -1500,7 +1515,7 @@
     </row>
     <row r="59">
       <c r="A59" t="s" s="4">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B59" t="s" s="4">
         <v>8</v>
@@ -1514,7 +1529,7 @@
     </row>
     <row r="60">
       <c r="A60" t="s" s="4">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B60" t="s" s="4">
         <v>8</v>
@@ -1528,7 +1543,7 @@
     </row>
     <row r="61">
       <c r="A61" t="s" s="4">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B61" t="s" s="4">
         <v>8</v>
@@ -1542,7 +1557,7 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="4">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B62" t="s" s="4">
         <v>8</v>
@@ -1556,7 +1571,7 @@
     </row>
     <row r="63">
       <c r="A63" t="s" s="4">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B63" t="s" s="4">
         <v>8</v>
@@ -1570,7 +1585,7 @@
     </row>
     <row r="64">
       <c r="A64" t="s" s="4">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B64" t="s" s="4">
         <v>8</v>
@@ -1584,7 +1599,7 @@
     </row>
     <row r="65">
       <c r="A65" t="s" s="4">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B65" t="s" s="4">
         <v>8</v>
@@ -1598,7 +1613,7 @@
     </row>
     <row r="66">
       <c r="A66" t="s" s="4">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B66" t="s" s="4">
         <v>8</v>
@@ -1612,7 +1627,7 @@
     </row>
     <row r="67">
       <c r="A67" t="s" s="4">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B67" t="s" s="4">
         <v>8</v>
@@ -1626,7 +1641,7 @@
     </row>
     <row r="68">
       <c r="A68" t="s" s="4">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B68" t="s" s="4">
         <v>8</v>
@@ -1640,7 +1655,7 @@
     </row>
     <row r="69">
       <c r="A69" t="s" s="4">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B69" t="s" s="4">
         <v>8</v>
@@ -1654,7 +1669,7 @@
     </row>
     <row r="70">
       <c r="A70" t="s" s="4">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B70" t="s" s="4">
         <v>8</v>
@@ -1668,7 +1683,7 @@
     </row>
     <row r="71">
       <c r="A71" t="s" s="4">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B71" t="s" s="4">
         <v>8</v>
@@ -1682,7 +1697,7 @@
     </row>
     <row r="72">
       <c r="A72" t="s" s="4">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B72" t="s" s="4">
         <v>8</v>
@@ -1696,7 +1711,7 @@
     </row>
     <row r="73">
       <c r="A73" t="s" s="4">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B73" t="s" s="4">
         <v>8</v>
@@ -1710,7 +1725,7 @@
     </row>
     <row r="74">
       <c r="A74" t="s" s="4">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B74" t="s" s="4">
         <v>8</v>
@@ -1724,7 +1739,7 @@
     </row>
     <row r="75">
       <c r="A75" t="s" s="4">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B75" t="s" s="4">
         <v>8</v>
@@ -1738,7 +1753,7 @@
     </row>
     <row r="76">
       <c r="A76" t="s" s="4">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B76" t="s" s="4">
         <v>8</v>
@@ -1752,7 +1767,7 @@
     </row>
     <row r="77">
       <c r="A77" t="s" s="4">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B77" t="s" s="4">
         <v>8</v>
@@ -1766,7 +1781,7 @@
     </row>
     <row r="78">
       <c r="A78" t="s" s="4">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B78" t="s" s="4">
         <v>8</v>
@@ -1780,7 +1795,7 @@
     </row>
     <row r="79">
       <c r="A79" t="s" s="4">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B79" t="s" s="4">
         <v>8</v>
@@ -1794,7 +1809,7 @@
     </row>
     <row r="80">
       <c r="A80" t="s" s="4">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B80" t="s" s="4">
         <v>8</v>
@@ -1808,7 +1823,7 @@
     </row>
     <row r="81">
       <c r="A81" t="s" s="4">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B81" t="s" s="4">
         <v>8</v>
@@ -1822,7 +1837,7 @@
     </row>
     <row r="82">
       <c r="A82" t="s" s="4">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B82" t="s" s="4">
         <v>8</v>
@@ -1836,21 +1851,21 @@
     </row>
     <row r="83">
       <c r="A83" t="s" s="4">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B83" t="s" s="4">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C83" t="s" s="4">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D83" t="s" s="4">
-        <v>10</v>
+        <v>95</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s" s="4">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B84" t="s" s="4">
         <v>8</v>
@@ -1864,7 +1879,7 @@
     </row>
     <row r="85">
       <c r="A85" t="s" s="4">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B85" t="s" s="4">
         <v>8</v>
@@ -1878,7 +1893,7 @@
     </row>
     <row r="86">
       <c r="A86" t="s" s="4">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B86" t="s" s="4">
         <v>8</v>
@@ -1892,7 +1907,7 @@
     </row>
     <row r="87">
       <c r="A87" t="s" s="4">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B87" t="s" s="4">
         <v>8</v>
@@ -1906,7 +1921,7 @@
     </row>
     <row r="88">
       <c r="A88" t="s" s="4">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B88" t="s" s="4">
         <v>8</v>
@@ -1920,7 +1935,7 @@
     </row>
     <row r="89">
       <c r="A89" t="s" s="4">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B89" t="s" s="4">
         <v>8</v>
@@ -1934,7 +1949,7 @@
     </row>
     <row r="90">
       <c r="A90" t="s" s="4">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B90" t="s" s="4">
         <v>8</v>
@@ -1948,7 +1963,7 @@
     </row>
     <row r="91">
       <c r="A91" t="s" s="4">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B91" t="s" s="4">
         <v>8</v>
@@ -1962,7 +1977,7 @@
     </row>
     <row r="92">
       <c r="A92" t="s" s="4">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B92" t="s" s="4">
         <v>8</v>
@@ -1976,7 +1991,7 @@
     </row>
     <row r="93">
       <c r="A93" t="s" s="4">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B93" t="s" s="4">
         <v>8</v>
@@ -1990,7 +2005,7 @@
     </row>
     <row r="94">
       <c r="A94" t="s" s="4">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B94" t="s" s="4">
         <v>8</v>
@@ -2004,7 +2019,7 @@
     </row>
     <row r="95">
       <c r="A95" t="s" s="4">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B95" t="s" s="4">
         <v>8</v>
@@ -2018,7 +2033,7 @@
     </row>
     <row r="96">
       <c r="A96" t="s" s="4">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B96" t="s" s="4">
         <v>8</v>
@@ -2032,7 +2047,7 @@
     </row>
     <row r="97">
       <c r="A97" t="s" s="4">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B97" t="s" s="4">
         <v>8</v>
@@ -2046,7 +2061,7 @@
     </row>
     <row r="98">
       <c r="A98" t="s" s="4">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B98" t="s" s="4">
         <v>8</v>
@@ -2060,7 +2075,7 @@
     </row>
     <row r="99">
       <c r="A99" t="s" s="4">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B99" t="s" s="4">
         <v>8</v>
@@ -2074,7 +2089,7 @@
     </row>
     <row r="100">
       <c r="A100" t="s" s="4">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B100" t="s" s="4">
         <v>8</v>
@@ -2088,7 +2103,7 @@
     </row>
     <row r="101">
       <c r="A101" t="s" s="4">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B101" t="s" s="4">
         <v>8</v>
@@ -2102,7 +2117,7 @@
     </row>
     <row r="102">
       <c r="A102" t="s" s="4">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B102" t="s" s="4">
         <v>8</v>
@@ -2116,7 +2131,7 @@
     </row>
     <row r="103">
       <c r="A103" t="s" s="4">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B103" t="s" s="4">
         <v>8</v>
@@ -2130,7 +2145,7 @@
     </row>
     <row r="104">
       <c r="A104" t="s" s="4">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B104" t="s" s="4">
         <v>8</v>
@@ -2144,7 +2159,7 @@
     </row>
     <row r="105">
       <c r="A105" t="s" s="4">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B105" t="s" s="4">
         <v>8</v>
@@ -2158,7 +2173,7 @@
     </row>
     <row r="106">
       <c r="A106" t="s" s="4">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B106" t="s" s="4">
         <v>8</v>
@@ -2172,7 +2187,7 @@
     </row>
     <row r="107">
       <c r="A107" t="s" s="4">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B107" t="s" s="4">
         <v>8</v>
@@ -2186,7 +2201,7 @@
     </row>
     <row r="108">
       <c r="A108" t="s" s="4">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B108" t="s" s="4">
         <v>8</v>
@@ -2200,7 +2215,7 @@
     </row>
     <row r="109">
       <c r="A109" t="s" s="4">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B109" t="s" s="4">
         <v>8</v>
@@ -2214,7 +2229,7 @@
     </row>
     <row r="110">
       <c r="A110" t="s" s="4">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B110" t="s" s="4">
         <v>8</v>
@@ -2228,7 +2243,7 @@
     </row>
     <row r="111">
       <c r="A111" t="s" s="4">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B111" t="s" s="4">
         <v>8</v>
@@ -2242,7 +2257,7 @@
     </row>
     <row r="112">
       <c r="A112" t="s" s="4">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B112" t="s" s="4">
         <v>8</v>
@@ -2256,7 +2271,7 @@
     </row>
     <row r="113">
       <c r="A113" t="s" s="4">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B113" t="s" s="4">
         <v>8</v>
@@ -2270,7 +2285,7 @@
     </row>
     <row r="114">
       <c r="A114" t="s" s="4">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B114" t="s" s="4">
         <v>8</v>
@@ -2284,7 +2299,7 @@
     </row>
     <row r="115">
       <c r="A115" t="s" s="4">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B115" t="s" s="4">
         <v>8</v>
@@ -2298,7 +2313,7 @@
     </row>
     <row r="116">
       <c r="A116" t="s" s="4">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B116" t="s" s="4">
         <v>8</v>
@@ -2312,7 +2327,7 @@
     </row>
     <row r="117">
       <c r="A117" t="s" s="3">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B117" t="s" s="3">
         <v>8</v>
@@ -2326,7 +2341,7 @@
     </row>
     <row r="118">
       <c r="A118" t="s" s="4">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B118" t="s" s="4">
         <v>8</v>
@@ -2340,7 +2355,7 @@
     </row>
     <row r="119">
       <c r="A119" t="s" s="4">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B119" t="s" s="4">
         <v>8</v>
@@ -2354,7 +2369,7 @@
     </row>
     <row r="120">
       <c r="A120" t="s" s="3">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B120" t="s" s="3">
         <v>8</v>
@@ -2368,7 +2383,7 @@
     </row>
     <row r="121">
       <c r="A121" t="s" s="4">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B121" t="s" s="4">
         <v>8</v>
@@ -2382,7 +2397,7 @@
     </row>
     <row r="122">
       <c r="A122" t="s" s="4">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B122" t="s" s="4">
         <v>8</v>
@@ -2396,7 +2411,7 @@
     </row>
     <row r="123">
       <c r="A123" t="s" s="4">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B123" t="s" s="4">
         <v>8</v>
@@ -2410,7 +2425,7 @@
     </row>
     <row r="124">
       <c r="A124" t="s" s="4">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B124" t="s" s="4">
         <v>8</v>
@@ -2424,7 +2439,7 @@
     </row>
     <row r="125">
       <c r="A125" t="s" s="4">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B125" t="s" s="4">
         <v>8</v>
@@ -2438,7 +2453,7 @@
     </row>
     <row r="126">
       <c r="A126" t="s" s="4">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B126" t="s" s="4">
         <v>8</v>
@@ -2452,7 +2467,7 @@
     </row>
     <row r="127">
       <c r="A127" t="s" s="4">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B127" t="s" s="4">
         <v>8</v>
@@ -2466,7 +2481,7 @@
     </row>
     <row r="128">
       <c r="A128" t="s" s="4">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B128" t="s" s="4">
         <v>8</v>
@@ -2480,7 +2495,7 @@
     </row>
     <row r="129">
       <c r="A129" t="s" s="4">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B129" t="s" s="4">
         <v>8</v>
@@ -2494,7 +2509,7 @@
     </row>
     <row r="130">
       <c r="A130" t="s" s="4">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B130" t="s" s="4">
         <v>8</v>
@@ -2508,21 +2523,21 @@
     </row>
     <row r="131">
       <c r="A131" t="s" s="4">
+        <v>143</v>
+      </c>
+      <c r="B131" t="s" s="4">
+        <v>48</v>
+      </c>
+      <c r="C131" t="s" s="4">
+        <v>145</v>
+      </c>
+      <c r="D131" t="s" s="4">
         <v>144</v>
-      </c>
-      <c r="B131" t="s" s="4">
-        <v>8</v>
-      </c>
-      <c r="C131" t="s" s="4">
-        <v>11</v>
-      </c>
-      <c r="D131" t="s" s="4">
-        <v>10</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="s" s="4">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B132" t="s" s="4">
         <v>8</v>
@@ -2536,7 +2551,7 @@
     </row>
     <row r="133">
       <c r="A133" t="s" s="4">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B133" t="s" s="4">
         <v>8</v>
@@ -2550,7 +2565,7 @@
     </row>
     <row r="134">
       <c r="A134" t="s" s="4">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B134" t="s" s="4">
         <v>8</v>
@@ -2564,7 +2579,7 @@
     </row>
     <row r="135">
       <c r="A135" t="s" s="4">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B135" t="s" s="4">
         <v>8</v>
@@ -2578,7 +2593,7 @@
     </row>
     <row r="136">
       <c r="A136" t="s" s="4">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B136" t="s" s="4">
         <v>8</v>
@@ -2592,7 +2607,7 @@
     </row>
     <row r="137">
       <c r="A137" t="s" s="4">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B137" t="s" s="4">
         <v>8</v>
@@ -2606,7 +2621,7 @@
     </row>
     <row r="138">
       <c r="A138" t="s" s="4">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B138" t="s" s="4">
         <v>8</v>
@@ -2620,7 +2635,7 @@
     </row>
     <row r="139">
       <c r="A139" t="s" s="4">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B139" t="s" s="4">
         <v>8</v>
@@ -2634,7 +2649,7 @@
     </row>
     <row r="140">
       <c r="A140" t="s" s="4">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B140" t="s" s="4">
         <v>8</v>
@@ -2648,7 +2663,7 @@
     </row>
     <row r="141">
       <c r="A141" t="s" s="4">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B141" t="s" s="4">
         <v>8</v>
@@ -2662,7 +2677,7 @@
     </row>
     <row r="142">
       <c r="A142" t="s" s="4">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B142" t="s" s="4">
         <v>8</v>
@@ -2676,7 +2691,7 @@
     </row>
     <row r="143">
       <c r="A143" t="s" s="4">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B143" t="s" s="4">
         <v>8</v>
@@ -2690,7 +2705,7 @@
     </row>
     <row r="144">
       <c r="A144" t="s" s="4">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B144" t="s" s="4">
         <v>8</v>
@@ -2704,7 +2719,7 @@
     </row>
     <row r="145">
       <c r="A145" t="s" s="4">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B145" t="s" s="4">
         <v>8</v>
@@ -2718,7 +2733,7 @@
     </row>
     <row r="146">
       <c r="A146" t="s" s="4">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B146" t="s" s="4">
         <v>8</v>
@@ -2732,7 +2747,7 @@
     </row>
     <row r="147">
       <c r="A147" t="s" s="4">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B147" t="s" s="4">
         <v>8</v>
@@ -2746,7 +2761,7 @@
     </row>
     <row r="148">
       <c r="A148" t="s" s="4">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B148" t="s" s="4">
         <v>8</v>
@@ -2760,7 +2775,7 @@
     </row>
     <row r="149">
       <c r="A149" t="s" s="4">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B149" t="s" s="4">
         <v>8</v>
@@ -2774,7 +2789,7 @@
     </row>
     <row r="150">
       <c r="A150" t="s" s="4">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B150" t="s" s="4">
         <v>8</v>
@@ -2788,7 +2803,7 @@
     </row>
     <row r="151">
       <c r="A151" t="s" s="4">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B151" t="s" s="4">
         <v>8</v>
@@ -2802,7 +2817,7 @@
     </row>
     <row r="152">
       <c r="A152" t="s" s="4">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B152" t="s" s="4">
         <v>8</v>
@@ -2816,7 +2831,7 @@
     </row>
     <row r="153">
       <c r="A153" t="s" s="4">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B153" t="s" s="4">
         <v>8</v>
@@ -2830,7 +2845,7 @@
     </row>
     <row r="154">
       <c r="A154" t="s" s="4">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B154" t="s" s="4">
         <v>8</v>
@@ -2844,7 +2859,7 @@
     </row>
     <row r="155">
       <c r="A155" t="s" s="4">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B155" t="s" s="4">
         <v>8</v>
@@ -2858,7 +2873,7 @@
     </row>
     <row r="156">
       <c r="A156" t="s" s="4">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B156" t="s" s="4">
         <v>8</v>
@@ -2872,7 +2887,7 @@
     </row>
     <row r="157">
       <c r="A157" t="s" s="4">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B157" t="s" s="4">
         <v>8</v>
@@ -2886,7 +2901,7 @@
     </row>
     <row r="158">
       <c r="A158" t="s" s="4">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B158" t="s" s="4">
         <v>8</v>
@@ -2900,7 +2915,7 @@
     </row>
     <row r="159">
       <c r="A159" t="s" s="4">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B159" t="s" s="4">
         <v>8</v>
@@ -2914,7 +2929,7 @@
     </row>
     <row r="160">
       <c r="A160" t="s" s="4">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B160" t="s" s="4">
         <v>8</v>
@@ -2928,7 +2943,7 @@
     </row>
     <row r="161">
       <c r="A161" t="s" s="4">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B161" t="s" s="4">
         <v>8</v>
@@ -2942,7 +2957,7 @@
     </row>
     <row r="162">
       <c r="A162" t="s" s="3">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B162" t="s" s="3">
         <v>8</v>
@@ -2956,7 +2971,7 @@
     </row>
     <row r="163">
       <c r="A163" t="s" s="4">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B163" t="s" s="4">
         <v>8</v>
@@ -2970,7 +2985,7 @@
     </row>
     <row r="164">
       <c r="A164" t="s" s="4">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B164" t="s" s="4">
         <v>8</v>
@@ -2984,7 +2999,7 @@
     </row>
     <row r="165">
       <c r="A165" t="s" s="4">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B165" t="s" s="4">
         <v>8</v>
@@ -2998,7 +3013,7 @@
     </row>
     <row r="166">
       <c r="A166" t="s" s="4">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B166" t="s" s="4">
         <v>8</v>
@@ -3012,7 +3027,7 @@
     </row>
     <row r="167">
       <c r="A167" t="s" s="4">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B167" t="s" s="4">
         <v>8</v>
@@ -3026,7 +3041,7 @@
     </row>
     <row r="168">
       <c r="A168" t="s" s="4">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B168" t="s" s="4">
         <v>8</v>
@@ -3040,7 +3055,7 @@
     </row>
     <row r="169">
       <c r="A169" t="s" s="4">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B169" t="s" s="4">
         <v>8</v>
@@ -3054,7 +3069,7 @@
     </row>
     <row r="170">
       <c r="A170" t="s" s="4">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B170" t="s" s="4">
         <v>8</v>
@@ -3068,7 +3083,7 @@
     </row>
     <row r="171">
       <c r="A171" t="s" s="4">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B171" t="s" s="4">
         <v>8</v>
@@ -3082,7 +3097,7 @@
     </row>
     <row r="172">
       <c r="A172" t="s" s="4">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B172" t="s" s="4">
         <v>8</v>
@@ -3096,7 +3111,7 @@
     </row>
     <row r="173">
       <c r="A173" t="s" s="4">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B173" t="s" s="4">
         <v>8</v>
@@ -3110,7 +3125,7 @@
     </row>
     <row r="174">
       <c r="A174" t="s" s="4">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B174" t="s" s="4">
         <v>8</v>
@@ -3124,7 +3139,7 @@
     </row>
     <row r="175">
       <c r="A175" t="s" s="4">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B175" t="s" s="4">
         <v>8</v>
@@ -3138,7 +3153,7 @@
     </row>
     <row r="176">
       <c r="A176" t="s" s="4">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B176" t="s" s="4">
         <v>8</v>
@@ -3152,7 +3167,7 @@
     </row>
     <row r="177">
       <c r="A177" t="s" s="4">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B177" t="s" s="4">
         <v>8</v>
@@ -3166,7 +3181,7 @@
     </row>
     <row r="178">
       <c r="A178" t="s" s="4">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B178" t="s" s="4">
         <v>8</v>
@@ -3180,7 +3195,7 @@
     </row>
     <row r="179">
       <c r="A179" t="s" s="4">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B179" t="s" s="4">
         <v>8</v>
@@ -3194,7 +3209,7 @@
     </row>
     <row r="180">
       <c r="A180" t="s" s="4">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B180" t="s" s="4">
         <v>8</v>
@@ -3208,7 +3223,7 @@
     </row>
     <row r="181">
       <c r="A181" t="s" s="4">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B181" t="s" s="4">
         <v>8</v>
@@ -3222,7 +3237,7 @@
     </row>
     <row r="182">
       <c r="A182" t="s" s="4">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B182" t="s" s="4">
         <v>8</v>
@@ -3236,7 +3251,7 @@
     </row>
     <row r="183">
       <c r="A183" t="s" s="4">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B183" t="s" s="4">
         <v>8</v>
@@ -3250,35 +3265,35 @@
     </row>
     <row r="184">
       <c r="A184" t="s" s="4">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B184" t="s" s="4">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C184" t="s" s="4">
-        <v>11</v>
+        <v>200</v>
       </c>
       <c r="D184" t="s" s="4">
-        <v>10</v>
+        <v>199</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="s" s="4">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B185" t="s" s="4">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C185" t="s" s="4">
-        <v>11</v>
+        <v>203</v>
       </c>
       <c r="D185" t="s" s="4">
-        <v>10</v>
+        <v>202</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="s" s="4">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="B186" t="s" s="4">
         <v>8</v>
@@ -3292,7 +3307,7 @@
     </row>
     <row r="187">
       <c r="A187" t="s" s="4">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B187" t="s" s="4">
         <v>8</v>
@@ -3306,7 +3321,7 @@
     </row>
     <row r="188">
       <c r="A188" t="s" s="4">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="B188" t="s" s="4">
         <v>8</v>
@@ -3320,7 +3335,7 @@
     </row>
     <row r="189">
       <c r="A189" t="s" s="4">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="B189" t="s" s="4">
         <v>8</v>
@@ -3334,7 +3349,7 @@
     </row>
     <row r="190">
       <c r="A190" t="s" s="4">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="B190" t="s" s="4">
         <v>8</v>

</xml_diff>